<commit_message>
Datos modificados en pruebas unitarias
</commit_message>
<xml_diff>
--- a/aDiary/usrdata/usuarios.xlsx
+++ b/aDiary/usrdata/usuarios.xlsx
@@ -12,30 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t/>
   </si>
   <si>
-    <t>Antonio</t>
+    <t>ahorasi</t>
   </si>
   <si>
-    <t>Fernando</t>
-  </si>
-  <si>
-    <t>Ayres</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Contraseña2</t>
-  </si>
-  <si>
-    <t>Dog</t>
-  </si>
-  <si>
-    <t>newDog</t>
+    <t>quesi</t>
   </si>
 </sst>
 </file>
@@ -90,7 +75,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -101,41 +86,16 @@
   </cols>
   <sheetData>
     <row customHeight="true" ht="12.8" r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
+      <c r="A2"/>
+      <c r="B2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Programa capaz de crear un propietario leyendo datos de excel.
</commit_message>
<xml_diff>
--- a/aDiary/usrdata/usuarios.xlsx
+++ b/aDiary/usrdata/usuarios.xlsx
@@ -12,15 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t/>
   </si>
   <si>
-    <t>ahorasi</t>
+    <t>Antonio</t>
   </si>
   <si>
-    <t>quesi</t>
+    <t>ctr</t>
+  </si>
+  <si>
+    <t>admin-Antonio</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>crt2</t>
   </si>
 </sst>
 </file>
@@ -75,7 +84,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -92,10 +101,22 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2"/>
       <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Implementaciones de las misiones en proyecto
</commit_message>
<xml_diff>
--- a/aDiary/usrdata/usuarios.xlsx
+++ b/aDiary/usrdata/usuarios.xlsx
@@ -12,24 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t/>
   </si>
   <si>
-    <t>Antonio</t>
+    <t>admin</t>
   </si>
   <si>
-    <t>ctr</t>
-  </si>
-  <si>
-    <t>admin-Antonio</t>
+    <t>default</t>
   </si>
   <si>
     <t>false</t>
   </si>
   <si>
-    <t>crt2</t>
+    <t>nuevo</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>admin-nuevo</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
@@ -99,24 +105,34 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>